<commit_message>
Implemented mapping logic for parsing manifests like the milestones. Refactored configurations for writing vs reading Excel
</commit_message>
<xml_diff>
--- a/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/milestones_INPUT.xlsx
+++ b/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/milestones_INPUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\controllers\journeys\delivery_planning\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F025C3A-C671-48D4-AA7A-383327FAC446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F140C739-058C-4BBD-AA24-B7EE59806EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{E0F713A6-EC14-46B4-BF9F-A256ED646BE0}"/>
   </bookViews>
@@ -822,7 +822,7 @@
   <dimension ref="B1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -939,7 +939,7 @@
         <v>58</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="9"/>
@@ -952,7 +952,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>13</v>
@@ -991,7 +991,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>15</v>
@@ -1020,7 +1020,7 @@
         <v>62</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="5"/>
@@ -1470,6 +1470,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FE2109BEF92BEF4C8E97B5AF946419EC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d28efe2c189899efa1786a30ea87be2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e212f830-3554-41ad-bc58-ca25e45c0c36" xmlns:ns3="ddeece39-a33c-49ad-a8fd-0ae9fa2c3195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0977d188311524f24189f8889752715f" ns2:_="" ns3:_="">
     <xsd:import namespace="e212f830-3554-41ad-bc58-ca25e45c0c36"/>
@@ -1680,15 +1689,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1696,6 +1696,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38F75AA3-BA7A-4A3B-B4CB-1B0EB08DC411}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1714,14 +1722,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8B96BA-B59D-47A4-B5CD-02C507056BD6}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Introduced JourneysController for some common functionality of all controllers in the Journeys domain
</commit_message>
<xml_diff>
--- a/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/milestones_INPUT.xlsx
+++ b/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/milestones_INPUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\controllers\journeys\delivery_planning\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F140C739-058C-4BBD-AA24-B7EE59806EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49436488-8B11-4B49-9086-E22BD66B6E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{E0F713A6-EC14-46B4-BF9F-A256ED646BE0}"/>
   </bookViews>
@@ -308,10 +308,10 @@
     <t>manifestAPI</t>
   </si>
   <si>
-    <t>milestone.journeys.a6i.io/v1</t>
-  </si>
-  <si>
     <t>knowledgeBase</t>
+  </si>
+  <si>
+    <t>delivery-planning.journeys.a6i.io/v1</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
   <dimension ref="B1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -857,7 +857,7 @@
         <v>90</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>59</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>9</v>
@@ -1470,15 +1470,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FE2109BEF92BEF4C8E97B5AF946419EC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d28efe2c189899efa1786a30ea87be2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e212f830-3554-41ad-bc58-ca25e45c0c36" xmlns:ns3="ddeece39-a33c-49ad-a8fd-0ae9fa2c3195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0977d188311524f24189f8889752715f" ns2:_="" ns3:_="">
     <xsd:import namespace="e212f830-3554-41ad-bc58-ca25e45c0c36"/>
@@ -1689,6 +1680,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1696,14 +1696,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38F75AA3-BA7A-4A3B-B4CB-1B0EB08DC411}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1722,6 +1714,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8B96BA-B59D-47A4-B5CD-02C507056BD6}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Partial progress with milestones form generation, fixing some unrelated bugs along the way
</commit_message>
<xml_diff>
--- a/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/milestones_INPUT.xlsx
+++ b/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/milestones_INPUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\controllers\journeys\delivery_planning\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49436488-8B11-4B49-9086-E22BD66B6E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849BD853-1BB0-479B-A614-2E0CB78F191F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{E0F713A6-EC14-46B4-BF9F-A256ED646BE0}"/>
   </bookViews>
@@ -311,7 +311,7 @@
     <t>knowledgeBase</t>
   </si>
   <si>
-    <t>delivery-planning.journeys.a6i.io/v1</t>
+    <t>delivery-planning.journeys.a6i.io/v1a</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
   <dimension ref="B1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1470,6 +1470,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FE2109BEF92BEF4C8E97B5AF946419EC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d28efe2c189899efa1786a30ea87be2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e212f830-3554-41ad-bc58-ca25e45c0c36" xmlns:ns3="ddeece39-a33c-49ad-a8fd-0ae9fa2c3195" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0977d188311524f24189f8889752715f" ns2:_="" ns3:_="">
     <xsd:import namespace="e212f830-3554-41ad-bc58-ca25e45c0c36"/>
@@ -1680,15 +1689,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1696,6 +1696,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38F75AA3-BA7A-4A3B-B4CB-1B0EB08DC411}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1714,14 +1722,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E56CA40E-146C-4986-9E85-E9ED557F93C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE8B96BA-B59D-47A4-B5CD-02C507056BD6}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Implemented support for multiple many-to-many relationships for a referencing manifest
</commit_message>
<xml_diff>
--- a/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/milestones_INPUT.xlsx
+++ b/src/apodeixi/controllers/journeys/delivery_planning/tests_unit/input_data/milestones_INPUT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\src\apodeixi\controllers\journeys\delivery_planning\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849BD853-1BB0-479B-A614-2E0CB78F191F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A12EDAA-D923-4885-A674-94ACA36A14BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{E0F713A6-EC14-46B4-BF9F-A256ED646BE0}"/>
   </bookViews>
@@ -230,9 +230,6 @@
     <t>FY 22</t>
   </si>
   <si>
-    <t>L2:P30</t>
-  </si>
-  <si>
     <t>Modernization milestone</t>
   </si>
   <si>
@@ -242,9 +239,6 @@
     <t>Sub Breakdown</t>
   </si>
   <si>
-    <t>E7:J50</t>
-  </si>
-  <si>
     <t>Opus Health Pro</t>
   </si>
   <si>
@@ -312,6 +306,12 @@
   </si>
   <si>
     <t>delivery-planning.journeys.a6i.io/v1a</t>
+  </si>
+  <si>
+    <t>E7:J28</t>
+  </si>
+  <si>
+    <t>L2:P28</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
   <dimension ref="B1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -854,10 +854,10 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>92</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>59</v>
@@ -869,7 +869,7 @@
         <v>20</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>28</v>
@@ -880,22 +880,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>22</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N3" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="16" t="s">
         <v>76</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="P3" s="16" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.45">
@@ -926,7 +926,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="9"/>
@@ -939,7 +939,7 @@
         <v>58</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="9"/>
@@ -952,7 +952,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>13</v>
@@ -970,7 +970,7 @@
         <v>13</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K7" s="12"/>
       <c r="M7" s="10" t="s">
@@ -980,7 +980,7 @@
         <v>20</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P7" s="10" t="s">
         <v>28</v>
@@ -991,7 +991,7 @@
         <v>61</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>15</v>
@@ -1003,7 +1003,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="15"/>
@@ -1020,7 +1020,7 @@
         <v>62</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="E9" s="8"/>
       <c r="F9" s="5"/>
@@ -1028,7 +1028,7 @@
         <v>1.2</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="15"/>
@@ -1045,7 +1045,7 @@
         <v>63</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="5"/>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>9</v>
@@ -1136,7 +1136,7 @@
         <v>2.1</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="15"/>
@@ -1153,7 +1153,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="5"/>
@@ -1161,7 +1161,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="15"/>
@@ -1186,7 +1186,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="15"/>
@@ -1203,7 +1203,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="5"/>
@@ -1346,13 +1346,13 @@
         <v>17</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G23" s="5">
         <v>3.1</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="15"/>
@@ -1371,7 +1371,7 @@
         <v>3.2</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="15"/>
@@ -1390,13 +1390,13 @@
         <v>3.3</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>43</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K25" s="13"/>
       <c r="M25" s="9" t="s">

</xml_diff>